<commit_message>
Add concentration, pH, and ingredient role support for chemical mixtures
This enhances the schema to better represent defined growth media and
other chemical mixtures with precise concentrations.

New classes:
- Concentration: value + unit for specifying amounts
- IngredientRole hierarchy: ElementSourceRole, BufferRole, SolventRole,
  NutrientRole, VitaminRole, MineralNutrientRole

New slots:
- ph: float (0-14) on ChemicalMixture
- concentration: Concentration object on ProportionalPart
- has_ingredient_role: structured role for ingredients
- source_element: for ElementSourceRole

New enum:
- ConcentrationUnitEnum: M, mM, uM, nM, g/L, mg/L, ug/L, ng/L,
  percent_w/v, percent_v/v, percent_w/w, ppm, ppb

Example:
- ImpreciseChemicalMixture-RCH2_alphaKG_medium.yaml demonstrating
  a bacterial growth medium from the Fitness Browser

@dragon-ai-agent

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/schema/excel/chemrof.xlsx
+++ b/schema/excel/chemrof.xlsx
@@ -75,26 +75,34 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AtomCation" sheetId="66" state="visible" r:id="rId66"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FullySpecifiedAtom" sheetId="67" state="visible" r:id="rId67"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="StandardInchiObject" sheetId="68" state="visible" r:id="rId68"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChemicalRole" sheetId="69" state="visible" r:id="rId69"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Stereocenter" sheetId="70" state="visible" r:id="rId70"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChiralityCenter" sheetId="71" state="visible" r:id="rId71"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AtomicBond" sheetId="72" state="visible" r:id="rId72"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SubatomicParticleOccurrence" sheetId="73" state="visible" r:id="rId73"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AtomOccurrence" sheetId="74" state="visible" r:id="rId74"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChemicalSalt" sheetId="75" state="visible" r:id="rId75"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ester" sheetId="76" state="visible" r:id="rId76"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Stereoisomer" sheetId="77" state="visible" r:id="rId77"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Enantiomer" sheetId="78" state="visible" r:id="rId78"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RacemicMixture" sheetId="79" state="visible" r:id="rId79"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Allotrope" sheetId="80" state="visible" r:id="rId80"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PolymerRepeatUnit" sheetId="81" state="visible" r:id="rId81"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Reaction" sheetId="82" state="visible" r:id="rId82"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="IsomeraseReaction" sheetId="83" state="visible" r:id="rId83"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ReactionParticipant" sheetId="84" state="visible" r:id="rId84"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ProportionalPart" sheetId="85" state="visible" r:id="rId85"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChemicalSimilarity" sheetId="86" state="visible" r:id="rId86"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MoleculePairwiseSimilarity" sheetId="87" state="visible" r:id="rId87"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TanimotoSimilarity" sheetId="88" state="visible" r:id="rId88"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Concentration" sheetId="69" state="visible" r:id="rId69"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChemicalRole" sheetId="70" state="visible" r:id="rId70"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="IngredientRole" sheetId="71" state="visible" r:id="rId71"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ElementSourceRole" sheetId="72" state="visible" r:id="rId72"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BufferRole" sheetId="73" state="visible" r:id="rId73"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SolventRole" sheetId="74" state="visible" r:id="rId74"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NutrientRole" sheetId="75" state="visible" r:id="rId75"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="VitaminRole" sheetId="76" state="visible" r:id="rId76"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MineralNutrientRole" sheetId="77" state="visible" r:id="rId77"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Stereocenter" sheetId="78" state="visible" r:id="rId78"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChiralityCenter" sheetId="79" state="visible" r:id="rId79"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AtomicBond" sheetId="80" state="visible" r:id="rId80"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SubatomicParticleOccurrence" sheetId="81" state="visible" r:id="rId81"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AtomOccurrence" sheetId="82" state="visible" r:id="rId82"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChemicalSalt" sheetId="83" state="visible" r:id="rId83"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ester" sheetId="84" state="visible" r:id="rId84"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Stereoisomer" sheetId="85" state="visible" r:id="rId85"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Enantiomer" sheetId="86" state="visible" r:id="rId86"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RacemicMixture" sheetId="87" state="visible" r:id="rId87"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Allotrope" sheetId="88" state="visible" r:id="rId88"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PolymerRepeatUnit" sheetId="89" state="visible" r:id="rId89"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Reaction" sheetId="90" state="visible" r:id="rId90"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="IsomeraseReaction" sheetId="91" state="visible" r:id="rId91"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ReactionParticipant" sheetId="92" state="visible" r:id="rId92"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ProportionalPart" sheetId="93" state="visible" r:id="rId93"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChemicalSimilarity" sheetId="94" state="visible" r:id="rId94"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MoleculePairwiseSimilarity" sheetId="95" state="visible" r:id="rId95"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TanimotoSimilarity" sheetId="96" state="visible" r:id="rId96"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1795,7 +1803,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:AB1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1806,135 +1814,140 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>ph</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>inchi_atom_connections_sublayer</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>IUPAC_name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>is_radical</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>has_chemical_role</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>inchi_string</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>inchi_chemical_sublayer</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>inchi_hydrogen_connections_sublayer</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>inchi_charge_sublayer</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>inchi_proton_sublayer</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>inchi_stereochemical_double_bond_sublayer</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>inchi_tetrahedral_stereochemical_sublayer</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>inchi_stereochemical_type_sublayer</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>inchi_isotopic_layer</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>smiles_string</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>empirical_formula</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>has_major_microspecies_at_pH7_3</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>molecular_mass</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>water_solubility</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>pka_ionization_constant</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>pka_temperature</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>pka_ionic_strength</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>pka_solvent</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>pka_pressure</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>owl_subclass_of</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
@@ -2736,7 +2749,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC1"/>
+  <dimension ref="A1:AD1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2757,135 +2770,140 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>ph</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>inchi_atom_connections_sublayer</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>IUPAC_name</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>is_radical</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>has_chemical_role</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>inchi_string</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>inchi_chemical_sublayer</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>inchi_hydrogen_connections_sublayer</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>inchi_charge_sublayer</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>inchi_proton_sublayer</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>inchi_stereochemical_double_bond_sublayer</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>inchi_tetrahedral_stereochemical_sublayer</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>inchi_stereochemical_type_sublayer</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>inchi_isotopic_layer</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>smiles_string</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>empirical_formula</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>has_major_microspecies_at_pH7_3</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>molecular_mass</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>water_solubility</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>pka_ionization_constant</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>pka_temperature</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>pka_ionic_strength</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>pka_solvent</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>pka_pressure</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>owl_subclass_of</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
@@ -4125,7 +4143,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD1"/>
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4151,135 +4169,140 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>ph</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>inchi_atom_connections_sublayer</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>IUPAC_name</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>is_radical</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>has_chemical_role</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>inchi_string</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>inchi_chemical_sublayer</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>inchi_hydrogen_connections_sublayer</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>inchi_charge_sublayer</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>inchi_proton_sublayer</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>inchi_stereochemical_double_bond_sublayer</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>inchi_tetrahedral_stereochemical_sublayer</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>inchi_stereochemical_type_sublayer</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>inchi_isotopic_layer</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>smiles_string</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>empirical_formula</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>has_major_microspecies_at_pH7_3</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>molecular_mass</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>water_solubility</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>pka_ionization_constant</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>pka_temperature</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>pka_ionic_strength</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>pka_solvent</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>pka_pressure</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>owl_subclass_of</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
@@ -9230,7 +9253,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9241,11 +9264,21 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>owl_subclass_of</t>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>unit</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"M,mM,uM,nM,g/L,mg/L,ug/L,ng/L,percent_w/v,percent_v/v,percent_w/w,ppm,ppb"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -9314,7 +9347,15 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>owl_subclass_of</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -9332,7 +9373,15 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>owl_subclass_of</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -9343,7 +9392,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9354,61 +9403,16 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>subject</t>
+          <t>source_element</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
-        <is>
-          <t>object</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>bond_type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>bond_order</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>bond_length</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>bond_energy</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>bond_length_in_angstroms</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>bond_angle</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>torsional_angle</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
         <is>
           <t>owl_subclass_of</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"covalent,aromatic,single,double,triple,quadruple,hydrogen,ionic,polycentric,metal-metal,salt bridge,polar covalent,sigma"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -9419,7 +9423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9429,16 +9433,6 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
-        <is>
-          <t>occurrence_of</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Count</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
         <is>
           <t>owl_subclass_of</t>
         </is>
@@ -9455,7 +9449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9465,36 +9459,6 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>occurrence_of</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>valence</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>oxidation_number</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>formal_charge</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>coordination_number</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
         <is>
           <t>owl_subclass_of</t>
         </is>
@@ -9511,7 +9475,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9522,137 +9486,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>inchi_atom_connections_sublayer</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>IUPAC_name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>is_radical</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_chemical_role</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>inchi_string</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>inchi_chemical_sublayer</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>inchi_hydrogen_connections_sublayer</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>inchi_charge_sublayer</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>inchi_proton_sublayer</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>inchi_stereochemical_double_bond_sublayer</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>inchi_tetrahedral_stereochemical_sublayer</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>inchi_stereochemical_type_sublayer</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>inchi_isotopic_layer</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>smiles_string</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>empirical_formula</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>has_major_microspecies_at_pH7_3</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>molecular_mass</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>water_solubility</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>pka_ionization_constant</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>pka_temperature</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>pka_ionic_strength</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>pka_solvent</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>pka_pressure</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
           <t>owl_subclass_of</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>type</t>
         </is>
       </c>
     </row>
@@ -9667,7 +9501,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9678,162 +9512,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>has_atom_occurrences</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>has_bonds</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>has_submolecules</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_atoms</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>is_organic</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>inchi_atom_connections_sublayer</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>IUPAC_name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>is_radical</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>has_chemical_role</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>inchi_string</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>inchi_chemical_sublayer</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>inchi_hydrogen_connections_sublayer</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>inchi_charge_sublayer</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>inchi_proton_sublayer</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>inchi_stereochemical_double_bond_sublayer</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>inchi_tetrahedral_stereochemical_sublayer</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>inchi_stereochemical_type_sublayer</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>inchi_isotopic_layer</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>smiles_string</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>empirical_formula</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>has_major_microspecies_at_pH7_3</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>molecular_mass</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>water_solubility</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>pka_ionization_constant</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>pka_temperature</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>pka_ionic_strength</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>pka_solvent</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>pka_pressure</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
           <t>owl_subclass_of</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>type</t>
         </is>
       </c>
     </row>
@@ -9848,7 +9527,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9859,162 +9538,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>has_atom_occurrences</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>has_bonds</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>has_submolecules</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_atoms</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>is_organic</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>inchi_atom_connections_sublayer</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>IUPAC_name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>is_radical</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>has_chemical_role</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>inchi_string</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>inchi_chemical_sublayer</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>inchi_hydrogen_connections_sublayer</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>inchi_charge_sublayer</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>inchi_proton_sublayer</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>inchi_stereochemical_double_bond_sublayer</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>inchi_tetrahedral_stereochemical_sublayer</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>inchi_stereochemical_type_sublayer</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>inchi_isotopic_layer</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>smiles_string</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>empirical_formula</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>has_major_microspecies_at_pH7_3</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>molecular_mass</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>water_solubility</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>pka_ionization_constant</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>pka_temperature</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>pka_ionic_strength</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>pka_solvent</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>pka_pressure</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
           <t>owl_subclass_of</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>type</t>
         </is>
       </c>
     </row>
@@ -10029,177 +9553,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>has_atom_occurrences</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>has_bonds</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>has_submolecules</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_atoms</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>is_organic</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>inchi_atom_connections_sublayer</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>IUPAC_name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>is_radical</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>has_chemical_role</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>inchi_string</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>inchi_chemical_sublayer</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>inchi_hydrogen_connections_sublayer</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>inchi_charge_sublayer</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>inchi_proton_sublayer</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>inchi_stereochemical_double_bond_sublayer</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>inchi_tetrahedral_stereochemical_sublayer</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>inchi_stereochemical_type_sublayer</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>inchi_isotopic_layer</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>smiles_string</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>empirical_formula</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>has_major_microspecies_at_pH7_3</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>molecular_mass</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>water_solubility</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>pka_ionization_constant</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>pka_temperature</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>pka_ionic_strength</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>pka_solvent</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>pka_pressure</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>owl_subclass_of</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -10210,167 +9571,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>has_left_enantiomer</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>has_right_enantiomer</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>chirality_agnostic_form</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>inchi_atom_connections_sublayer</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>IUPAC_name</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>is_radical</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>has_chemical_role</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>inchi_string</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>inchi_chemical_sublayer</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>inchi_hydrogen_connections_sublayer</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>inchi_charge_sublayer</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>inchi_proton_sublayer</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>inchi_stereochemical_double_bond_sublayer</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>inchi_tetrahedral_stereochemical_sublayer</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>inchi_stereochemical_type_sublayer</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>inchi_isotopic_layer</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>smiles_string</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>empirical_formula</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>has_major_microspecies_at_pH7_3</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>molecular_mass</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>water_solubility</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>pka_ionization_constant</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>pka_temperature</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>pka_ionic_strength</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>pka_solvent</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>pka_pressure</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>owl_subclass_of</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -10437,7 +9645,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10448,166 +9656,61 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>has_atom_occurrences</t>
+          <t>subject</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>has_bonds</t>
+          <t>object</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>has_submolecules</t>
+          <t>bond_type</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>has_atoms</t>
+          <t>bond_order</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>is_organic</t>
+          <t>bond_length</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>inchi_atom_connections_sublayer</t>
+          <t>bond_energy</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>IUPAC_name</t>
+          <t>bond_length_in_angstroms</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>is_radical</t>
+          <t>bond_angle</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>has_chemical_role</t>
+          <t>torsional_angle</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>inchi_string</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>inchi_chemical_sublayer</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>inchi_hydrogen_connections_sublayer</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>inchi_charge_sublayer</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>inchi_proton_sublayer</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>inchi_stereochemical_double_bond_sublayer</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>inchi_tetrahedral_stereochemical_sublayer</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>inchi_stereochemical_type_sublayer</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>inchi_isotopic_layer</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>smiles_string</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>empirical_formula</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>has_major_microspecies_at_pH7_3</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>molecular_mass</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>water_solubility</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>pka_ionization_constant</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>pka_temperature</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>pka_ionic_strength</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>pka_solvent</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>pka_pressure</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
           <t>owl_subclass_of</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>type</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"covalent,aromatic,single,double,triple,quadruple,hydrogen,ionic,polycentric,metal-metal,salt bridge,polar covalent,sigma"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -10618,7 +9721,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10628,6 +9731,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
+        <is>
+          <t>occurrence_of</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
         <is>
           <t>owl_subclass_of</t>
         </is>
@@ -10644,7 +9757,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10655,87 +9768,37 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>left_participants</t>
+          <t>name</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>right_participants</t>
+          <t>occurrence_of</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>direction</t>
+          <t>valence</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>is_diastereoselective</t>
+          <t>oxidation_number</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>is_stereo</t>
+          <t>formal_charge</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>is_balanced</t>
+          <t>coordination_number</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>is_transport</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>is_fully_characterized</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>reaction_center</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>has_rinchi_representation</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>has_reaction_smiles_representation</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>reaction_rate_coefficient</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>reaction_rate</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>reaction_type</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>type</t>
+          <t>owl_subclass_of</t>
         </is>
       </c>
     </row>
@@ -10750,7 +9813,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:AB1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10761,85 +9824,140 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>left_participants</t>
+          <t>ph</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>right_participants</t>
+          <t>inchi_atom_connections_sublayer</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>direction</t>
+          <t>IUPAC_name</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>is_diastereoselective</t>
+          <t>is_radical</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>is_stereo</t>
+          <t>has_chemical_role</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>is_balanced</t>
+          <t>inchi_string</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>is_transport</t>
+          <t>inchi_chemical_sublayer</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>is_fully_characterized</t>
+          <t>inchi_hydrogen_connections_sublayer</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>reaction_center</t>
+          <t>inchi_charge_sublayer</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>has_rinchi_representation</t>
+          <t>inchi_proton_sublayer</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>has_reaction_smiles_representation</t>
+          <t>inchi_stereochemical_double_bond_sublayer</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>reaction_rate_coefficient</t>
+          <t>inchi_tetrahedral_stereochemical_sublayer</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>reaction_rate</t>
+          <t>inchi_stereochemical_type_sublayer</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>reaction_type</t>
+          <t>inchi_isotopic_layer</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
+          <t>smiles_string</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>empirical_formula</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>has_major_microspecies_at_pH7_3</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>molecular_mass</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>water_solubility</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>pka_ionization_constant</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>pka_temperature</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>pka_ionic_strength</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>pka_solvent</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>pka_pressure</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>owl_subclass_of</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
@@ -10856,7 +9974,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:AF1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10867,7 +9985,162 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>has_atom_occurrences</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_bonds</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>has_submolecules</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_atoms</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>is_organic</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>inchi_atom_connections_sublayer</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>IUPAC_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>is_radical</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>has_chemical_role</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>inchi_string</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>inchi_chemical_sublayer</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>inchi_hydrogen_connections_sublayer</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>inchi_charge_sublayer</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>inchi_proton_sublayer</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>inchi_stereochemical_double_bond_sublayer</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>inchi_tetrahedral_stereochemical_sublayer</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>inchi_stereochemical_type_sublayer</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>inchi_isotopic_layer</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>smiles_string</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>empirical_formula</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>has_major_microspecies_at_pH7_3</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>molecular_mass</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>water_solubility</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>pka_ionization_constant</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>pka_temperature</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>pka_ionic_strength</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>pka_solvent</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>pka_pressure</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
           <t>owl_subclass_of</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>type</t>
         </is>
       </c>
     </row>
@@ -10882,7 +10155,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:AF1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10893,7 +10166,162 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>has_atom_occurrences</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_bonds</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>has_submolecules</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_atoms</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>is_organic</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>inchi_atom_connections_sublayer</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>IUPAC_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>is_radical</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>has_chemical_role</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>inchi_string</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>inchi_chemical_sublayer</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>inchi_hydrogen_connections_sublayer</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>inchi_charge_sublayer</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>inchi_proton_sublayer</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>inchi_stereochemical_double_bond_sublayer</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>inchi_tetrahedral_stereochemical_sublayer</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>inchi_stereochemical_type_sublayer</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>inchi_isotopic_layer</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>smiles_string</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>empirical_formula</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>has_major_microspecies_at_pH7_3</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>molecular_mass</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>water_solubility</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>pka_ionization_constant</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>pka_temperature</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>pka_ionic_strength</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>pka_solvent</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>pka_pressure</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
           <t>owl_subclass_of</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>type</t>
         </is>
       </c>
     </row>
@@ -10908,7 +10336,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:AF1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10919,7 +10347,162 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>has_atom_occurrences</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_bonds</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>has_submolecules</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_atoms</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>is_organic</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>inchi_atom_connections_sublayer</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>IUPAC_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>is_radical</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>has_chemical_role</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>inchi_string</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>inchi_chemical_sublayer</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>inchi_hydrogen_connections_sublayer</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>inchi_charge_sublayer</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>inchi_proton_sublayer</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>inchi_stereochemical_double_bond_sublayer</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>inchi_tetrahedral_stereochemical_sublayer</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>inchi_stereochemical_type_sublayer</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>inchi_isotopic_layer</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>smiles_string</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>empirical_formula</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>has_major_microspecies_at_pH7_3</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>molecular_mass</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>water_solubility</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>pka_ionization_constant</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>pka_temperature</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>pka_ionic_strength</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>pka_solvent</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>pka_pressure</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
           <t>owl_subclass_of</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>type</t>
         </is>
       </c>
     </row>
@@ -10934,7 +10517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10945,7 +10528,157 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>has_left_enantiomer</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_right_enantiomer</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>chirality_agnostic_form</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>ph</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>inchi_atom_connections_sublayer</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>IUPAC_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>is_radical</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>has_chemical_role</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>inchi_string</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>inchi_chemical_sublayer</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>inchi_hydrogen_connections_sublayer</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>inchi_charge_sublayer</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>inchi_proton_sublayer</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>inchi_stereochemical_double_bond_sublayer</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>inchi_tetrahedral_stereochemical_sublayer</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>inchi_stereochemical_type_sublayer</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>inchi_isotopic_layer</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>smiles_string</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>empirical_formula</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>has_major_microspecies_at_pH7_3</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>molecular_mass</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>water_solubility</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>pka_ionization_constant</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>pka_temperature</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>pka_ionic_strength</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>pka_solvent</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>pka_pressure</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
           <t>owl_subclass_of</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>type</t>
         </is>
       </c>
     </row>
@@ -10955,6 +10688,187 @@
 </file>
 
 <file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AF1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_atom_occurrences</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_bonds</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>has_submolecules</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_atoms</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>is_organic</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>inchi_atom_connections_sublayer</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>IUPAC_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>is_radical</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>has_chemical_role</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>inchi_string</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>inchi_chemical_sublayer</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>inchi_hydrogen_connections_sublayer</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>inchi_charge_sublayer</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>inchi_proton_sublayer</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>inchi_stereochemical_double_bond_sublayer</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>inchi_tetrahedral_stereochemical_sublayer</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>inchi_stereochemical_type_sublayer</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>inchi_isotopic_layer</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>smiles_string</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>empirical_formula</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>has_major_microspecies_at_pH7_3</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>molecular_mass</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>water_solubility</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>pka_ionization_constant</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>pka_temperature</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>pka_ionic_strength</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>pka_solvent</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>pka_pressure</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>owl_subclass_of</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -11034,4 +10948,356 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet90.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>left_participants</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>right_participants</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>direction</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>is_diastereoselective</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>is_stereo</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>is_balanced</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>is_transport</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>is_fully_characterized</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>reaction_center</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>has_rinchi_representation</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>has_reaction_smiles_representation</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>reaction_rate_coefficient</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>reaction_rate</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>reaction_type</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>left_participants</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>right_participants</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>direction</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>is_diastereoselective</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>is_stereo</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>is_balanced</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>is_transport</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>is_fully_characterized</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>reaction_center</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>has_rinchi_representation</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>has_reaction_smiles_representation</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>reaction_rate_coefficient</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>reaction_rate</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>reaction_type</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet92.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>owl_subclass_of</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet93.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_ingredient_role</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>concentration</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>owl_subclass_of</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>owl_subclass_of</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet95.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>owl_subclass_of</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet96.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>owl_subclass_of</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add IngredientRoleTypeEnum and update example with structured roles
- Add IngredientRoleTypeEnum with values: carbon_source, nitrogen_source,
  phosphorus_source, sulfur_source, electron_donor/acceptor, buffer,
  solvent, vitamin, mineral, trace_element, growth_factor, antibiotic,
  inducer, substrate
- Add role_type attribute to IngredientRole class
- Move source_element slot to IngredientRole base class for flexibility
- Update RCH2 medium example to demonstrate has_ingredient_role with
  role_type and source_element for element sources

@dragon-ai-agent

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/schema/excel/chemrof.xlsx
+++ b/schema/excel/chemrof.xlsx
@@ -9366,7 +9366,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9377,11 +9377,26 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>source_element</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>role_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>owl_subclass_of</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"carbon_source,nitrogen_source,phosphorus_source,sulfur_source,electron_donor,electron_acceptor,buffer,solvent,vitamin,mineral,trace_element,growth_factor,antibiotic,inducer,substrate"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -9392,7 +9407,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9408,11 +9423,21 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>role_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>owl_subclass_of</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"carbon_source,nitrogen_source,phosphorus_source,sulfur_source,electron_donor,electron_acceptor,buffer,solvent,vitamin,mineral,trace_element,growth_factor,antibiotic,inducer,substrate"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -9423,7 +9448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9434,11 +9459,26 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>source_element</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>role_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>owl_subclass_of</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"carbon_source,nitrogen_source,phosphorus_source,sulfur_source,electron_donor,electron_acceptor,buffer,solvent,vitamin,mineral,trace_element,growth_factor,antibiotic,inducer,substrate"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -9449,7 +9489,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9460,11 +9500,26 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>source_element</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>role_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>owl_subclass_of</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"carbon_source,nitrogen_source,phosphorus_source,sulfur_source,electron_donor,electron_acceptor,buffer,solvent,vitamin,mineral,trace_element,growth_factor,antibiotic,inducer,substrate"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -9475,7 +9530,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9486,11 +9541,26 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>source_element</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>role_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>owl_subclass_of</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"carbon_source,nitrogen_source,phosphorus_source,sulfur_source,electron_donor,electron_acceptor,buffer,solvent,vitamin,mineral,trace_element,growth_factor,antibiotic,inducer,substrate"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -9501,7 +9571,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9512,11 +9582,26 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>source_element</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>role_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>owl_subclass_of</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"carbon_source,nitrogen_source,phosphorus_source,sulfur_source,electron_donor,electron_acceptor,buffer,solvent,vitamin,mineral,trace_element,growth_factor,antibiotic,inducer,substrate"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -9527,7 +9612,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9538,11 +9623,26 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>source_element</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>role_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>owl_subclass_of</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"carbon_source,nitrogen_source,phosphorus_source,sulfur_source,electron_donor,electron_acceptor,buffer,solvent,vitamin,mineral,trace_element,growth_factor,antibiotic,inducer,substrate"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -11194,7 +11294,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11205,21 +11305,46 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>composed_of</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_role</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>has_ingredient_role</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>concentration</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>minimal_percentage</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>maximum_percentage</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
         <is>
           <t>owl_subclass_of</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"active ingredient,inactive ingredient,excipient,solvent"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>